<commit_message>
Update ORAICAN tracker via Streamlit
</commit_message>
<xml_diff>
--- a/oraican tracker.xlsx
+++ b/oraican tracker.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7876A2F9-C569-4295-BE83-8DF33CE31C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
     <sheet name="Meetings" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -41,6 +35,21 @@
     <t>Created</t>
   </si>
   <si>
+    <t>ee8eff1d-5687-4078-aca9-93064be1b736</t>
+  </si>
+  <si>
+    <t>test fetch push</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>2025-05-24</t>
+  </si>
+  <si>
+    <t>2025-05-24 08:52:36</t>
+  </si>
+  <si>
     <t>Topic</t>
   </si>
   <si>
@@ -51,13 +60,28 @@
   </si>
   <si>
     <t>Link</t>
+  </si>
+  <si>
+    <t>4bc1a0e8-c006-4711-9fcd-758da03917f6</t>
+  </si>
+  <si>
+    <t>test meeting / fetch push</t>
+  </si>
+  <si>
+    <t>10:00</t>
+  </si>
+  <si>
+    <t>https://meet.google.com/landing</t>
+  </si>
+  <si>
+    <t>2025-05-24 08:52:58</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,21 +157,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -185,7 +201,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -219,7 +235,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -254,10 +269,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -430,16 +444,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -457,6 +469,23 @@
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -465,45 +494,57 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E5" s="2"/>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>